<commit_message>
Legge immagini da celle con url
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/img_template.xlsx
+++ b/src/main/resources/excel/img_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC9CB27-A00F-4DEC-9979-9854CE0E2CE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2E83A7-777D-4159-AD36-E579F284D6C3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="3285" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="3090" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="C6")</t>
+jx:area(lastCell="D12")</t>
         </r>
       </text>
     </comment>
@@ -69,7 +69,55 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:image(lastCell="C6" src="image" imageType="PNG")</t>
+jx:image(lastCell="B4" src="image" imageType="PNG")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{4EC83F15-E5AC-49B1-8ED5-F90EDD14ADA2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:image(lastCell="B6" src="imageFromUrl" imageType="PNG")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{2D390BC6-4789-4168-B8B2-2FB74E391BA9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:image(lastCell="B11" src="https://linvitatospeciale.it/wp-content/uploads/2019/05/smeup.png" imageType="PNG")</t>
         </r>
       </text>
     </comment>
@@ -78,16 +126,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>ImageDemo</t>
+  </si>
+  <si>
+    <t>${url}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +165,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -419,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,6 +497,13 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>